<commit_message>
solved, but might still need some tweaking
</commit_message>
<xml_diff>
--- a/Temp/Customer Service Business Queue.xlsx
+++ b/Temp/Customer Service Business Queue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -34,7 +34,7 @@
     <x:t>Critical</x:t>
   </x:si>
   <x:si>
-    <x:t>Fred</x:t>
+    <x:t>Carol</x:t>
   </x:si>
   <x:si>
     <x:t>23.03.2018</x:t>
@@ -43,63 +43,57 @@
     <x:t>2. CSB1005</x:t>
   </x:si>
   <x:si>
+    <x:t>05.04.2018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3. CSB1007</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27.03.2018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4. CSB1019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>03.04.2018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5. CSB1030</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Low</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29.03.2018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6. CSB1033</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7. CSB1038</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01.04.2018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8. CSB1045</x:t>
+  </x:si>
+  <x:si>
+    <x:t>High</x:t>
+  </x:si>
+  <x:si>
+    <x:t>28.03.2018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9. CSB1048</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10. CSB1050</x:t>
+  </x:si>
+  <x:si>
     <x:t>Normal</x:t>
   </x:si>
   <x:si>
-    <x:t>Peter</x:t>
-  </x:si>
-  <x:si>
-    <x:t>05.04.2018</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3. CSB1007</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Carol</x:t>
-  </x:si>
-  <x:si>
-    <x:t>27.03.2018</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4. CSB1019</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Low</x:t>
-  </x:si>
-  <x:si>
-    <x:t>03.04.2018</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5. CSB1030</x:t>
-  </x:si>
-  <x:si>
-    <x:t>29.03.2018</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6. CSB1033</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7. CSB1038</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01.04.2018</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8. CSB1045</x:t>
-  </x:si>
-  <x:si>
-    <x:t>High</x:t>
-  </x:si>
-  <x:si>
-    <x:t>28.03.2018</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9. CSB1048</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10. CSB1050</x:t>
-  </x:si>
-  <x:si>
     <x:t>11. CSB1062</x:t>
   </x:si>
   <x:si>
@@ -110,12 +104,6 @@
   </x:si>
   <x:si>
     <x:t>13. CSB1066</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Very low</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Morgan</x:t>
   </x:si>
   <x:si>
     <x:t>30.03.2018</x:t>
@@ -538,74 +526,74 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
         <x:v>9</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="A4" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="A5" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4">
       <x:c r="A6" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
         <x:v>16</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4">
       <x:c r="A7" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:4">
       <x:c r="A8" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
         <x:v>5</x:v>
@@ -614,217 +602,217 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4">
       <x:c r="A9" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4">
       <x:c r="A10" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4">
       <x:c r="A11" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4">
       <x:c r="A12" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4">
       <x:c r="A13" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4">
       <x:c r="A14" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4">
       <x:c r="A15" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4">
       <x:c r="A16" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
       <x:c r="A17" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:4">
       <x:c r="A18" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4">
       <x:c r="A19" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4">
       <x:c r="A20" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:4">
       <x:c r="A21" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:4">
       <x:c r="A22" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:4">
       <x:c r="A23" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>